<commit_message>
Updates through the themes, need to discuss those in person I think.
</commit_message>
<xml_diff>
--- a/Tables_and_Graphs.xlsx
+++ b/Tables_and_Graphs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27928"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20414"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\matth\Desktop\PhD\Oral-Exam-Project-\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jbpost2\repos\Oral-Exam-Project-\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79DA3FDD-A393-477B-8DC5-87F32A8E07C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2760BA0C-A55F-432F-A31E-90B1D1ABFB68}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9510" yWindow="0" windowWidth="9780" windowHeight="11370" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9516" yWindow="0" windowWidth="9780" windowHeight="11376" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,10 +25,10 @@
         <xcalcf:feature name="microsoft.com:RD"/>
         <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -412,13 +412,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D43"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="D40" sqref="D40"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>8</v>
       </c>
@@ -432,7 +432,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>9</v>
       </c>
@@ -446,7 +446,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>9</v>
       </c>
@@ -460,7 +460,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>9</v>
       </c>
@@ -475,7 +475,7 @@
         <v>0.66666666666666663</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>9</v>
       </c>
@@ -490,7 +490,7 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -505,7 +505,7 @@
         <v>0.16666666666666666</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>9</v>
       </c>
@@ -520,7 +520,7 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>9</v>
       </c>
@@ -531,7 +531,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>9</v>
       </c>
@@ -546,7 +546,7 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -561,7 +561,7 @@
         <v>0.16666666666666666</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>10</v>
       </c>
@@ -572,7 +572,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -583,7 +583,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>10</v>
       </c>
@@ -594,7 +594,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>10</v>
       </c>
@@ -605,7 +605,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -616,7 +616,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>10</v>
       </c>
@@ -631,7 +631,7 @@
         <v>0.16666666666666666</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>10</v>
       </c>
@@ -642,7 +642,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>10</v>
       </c>
@@ -657,7 +657,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>10</v>
       </c>
@@ -672,7 +672,7 @@
         <v>0.16666666666666666</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>10</v>
       </c>
@@ -687,7 +687,7 @@
         <v>0.16666666666666666</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>10</v>
       </c>
@@ -701,7 +701,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>10</v>
       </c>
@@ -716,7 +716,7 @@
         <v>0.16666666666666666</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>10</v>
       </c>
@@ -727,7 +727,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>10</v>
       </c>
@@ -738,7 +738,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>10</v>
       </c>
@@ -749,7 +749,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>10</v>
       </c>
@@ -760,7 +760,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>10</v>
       </c>
@@ -775,7 +775,7 @@
         <v>0.16666666666666666</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>10</v>
       </c>
@@ -786,7 +786,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>10</v>
       </c>
@@ -801,7 +801,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>10</v>
       </c>
@@ -816,7 +816,7 @@
         <v>0.16666666666666666</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>10</v>
       </c>
@@ -827,7 +827,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>10</v>
       </c>
@@ -842,7 +842,7 @@
         <v>0.16666666666666666</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>10</v>
       </c>
@@ -853,7 +853,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>10</v>
       </c>
@@ -864,7 +864,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>10</v>
       </c>
@@ -875,7 +875,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>10</v>
       </c>
@@ -890,7 +890,7 @@
         <v>0.16666666666666666</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>10</v>
       </c>
@@ -901,7 +901,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>10</v>
       </c>
@@ -916,7 +916,7 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>10</v>
       </c>
@@ -931,7 +931,7 @@
         <v>0.33333333333333331</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>10</v>
       </c>
@@ -941,12 +941,8 @@
       <c r="C40">
         <v>10</v>
       </c>
-      <c r="D40">
-        <f>1/6</f>
-        <v>0.16666666666666666</v>
-      </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>14</v>
       </c>
@@ -961,7 +957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>14</v>
       </c>
@@ -976,7 +972,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>14</v>
       </c>

</xml_diff>